<commit_message>
Kleine verbeteringen aan de NS commando output
- correcte datum- opmaak verfijnd
</commit_message>
<xml_diff>
--- a/clanoverview_logs/generated_reports/2017-12-21_clanlog.xlsx
+++ b/clanoverview_logs/generated_reports/2017-12-21_clanlog.xlsx
@@ -170,19 +170,19 @@
     <t>#8U09PR0V</t>
   </si>
   <si>
+    <t>Bastos</t>
+  </si>
+  <si>
+    <t>#8RP8QV8V</t>
+  </si>
+  <si>
+    <t>member</t>
+  </si>
+  <si>
     <t>(j)de tik(j)</t>
   </si>
   <si>
     <t>#GYVQ0Y8R</t>
-  </si>
-  <si>
-    <t>Bastos</t>
-  </si>
-  <si>
-    <t>#8RP8QV8V</t>
-  </si>
-  <si>
-    <t>member</t>
   </si>
   <si>
     <t>pamuk39</t>
@@ -532,13 +532,13 @@
         <v>14</v>
       </c>
       <c r="G5" s="3" t="n">
-        <v>1192.0</v>
+        <v>1276.0</v>
       </c>
       <c r="H5" s="3" t="n">
         <v>2005.0</v>
       </c>
       <c r="I5" s="3" t="n">
-        <v>0.59</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="6">
@@ -584,7 +584,7 @@
         <v>184.0</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>5063.0</v>
+        <v>5066.0</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>14</v>
@@ -593,10 +593,10 @@
         <v>1889.0</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>1386.0</v>
+        <v>1423.0</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>1.36</v>
+        <v>1.33</v>
       </c>
     </row>
     <row r="8">
@@ -796,7 +796,7 @@
         <v>3374.0</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>3667.0</v>
+        <v>3674.0</v>
       </c>
       <c r="I14" s="2" t="n">
         <v>0.92</v>
@@ -1016,22 +1016,22 @@
         <v>53</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>178.0</v>
+        <v>172.0</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>4556.0</v>
+        <v>4555.0</v>
       </c>
       <c r="F22" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="G22" s="2" t="n">
-        <v>614.0</v>
+        <v>37.0</v>
       </c>
       <c r="H22" s="2" t="n">
-        <v>1624.0</v>
+        <v>0.0</v>
       </c>
       <c r="I22" s="2" t="n">
-        <v>0.38</v>
+        <v>37.0</v>
       </c>
     </row>
     <row r="23">
@@ -1039,28 +1039,28 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D23" s="3" t="n">
-        <v>172.0</v>
+        <v>178.0</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>4555.0</v>
+        <v>4554.0</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="G23" s="3" t="n">
-        <v>37.0</v>
+        <v>614.0</v>
       </c>
       <c r="H23" s="3" t="n">
-        <v>0.0</v>
+        <v>1624.0</v>
       </c>
       <c r="I23" s="3" t="n">
-        <v>37.0</v>
+        <v>0.38</v>
       </c>
     </row>
     <row r="24">
@@ -1167,7 +1167,7 @@
         <v>4392.0</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G27" s="3" t="n">
         <v>1095.0</v>
@@ -1193,7 +1193,7 @@
         <v>175.0</v>
       </c>
       <c r="E28" s="2" t="n">
-        <v>4334.0</v>
+        <v>4336.0</v>
       </c>
       <c r="F28" t="s">
         <v>14</v>
@@ -1202,10 +1202,10 @@
         <v>3167.0</v>
       </c>
       <c r="H28" s="2" t="n">
-        <v>3966.0</v>
+        <v>4001.0</v>
       </c>
       <c r="I28" s="2" t="n">
-        <v>0.8</v>
+        <v>0.79</v>
       </c>
     </row>
     <row r="29">
@@ -1254,7 +1254,7 @@
         <v>4099.0</v>
       </c>
       <c r="F30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G30" s="2" t="n">
         <v>68.0</v>
@@ -1283,7 +1283,7 @@
         <v>4041.0</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G31" s="3" t="n">
         <v>424.0</v>
@@ -1376,7 +1376,7 @@
         <v>7611.0</v>
       </c>
       <c r="H34" s="2" t="n">
-        <v>5763.0</v>
+        <v>5768.0</v>
       </c>
       <c r="I34" s="2" t="n">
         <v>1.32</v>
@@ -1399,7 +1399,7 @@
         <v>3605.0</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G35" s="3" t="n">
         <v>190.0</v>
@@ -1428,7 +1428,7 @@
         <v>3508.0</v>
       </c>
       <c r="F36" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G36" s="2" t="n">
         <v>1401.0</v>
@@ -1457,7 +1457,7 @@
         <v>3480.0</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G37" s="3" t="n">
         <v>853.0</v>
@@ -1573,7 +1573,7 @@
         <v>3109.0</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G41" s="3" t="n">
         <v>1343.0</v>
@@ -1631,7 +1631,7 @@
         <v>1347.0</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G43" s="3" t="n">
         <v>0.0</v>
@@ -1646,7 +1646,7 @@
   </sheetData>
   <pageMargins bottom="0.5" footer="0.3" header="0.3" left="0.25" right="0.25" top="0.5"/>
   <headerFooter>
-    <oddFooter>&amp;LClanoverzicht&amp;R21/12/2017 08:32</oddFooter>
+    <oddFooter>&amp;LClanoverzicht&amp;R21/12/2017 08:57</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>